<commit_message>
Build connection matrix F
</commit_message>
<xml_diff>
--- a/Task2/Input/Problem 2 data.xlsx
+++ b/Task2/Input/Problem 2 data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frederikedvardsen/Desktop/4. semester/TET4185 Kraftmarkeder, ressurs og miljø/Prosjekt/Task2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frederikedvardsen/Desktop/4. semester/TET4185 Kraftmarkeder, ressurs og miljø/Prosjekt/Task2/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090EBE0F-9F2C-3443-B66E-8AFCBBF15620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44AB625-FC6E-2541-A507-A83FCC3D6503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -472,7 +472,7 @@
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -679,7 +679,7 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Generalize find_params to n generators and loads
</commit_message>
<xml_diff>
--- a/Task2/Input/Problem 2 data.xlsx
+++ b/Task2/Input/Problem 2 data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frederikedvardsen/Desktop/4. semester/TET4185 Kraftmarkeder, ressurs og miljø/Prosjekt/Task2/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD357B9D-9685-CF4F-8B21-7D73B7610D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1072C8-9FEA-134A-BA9C-AAEFAEEA032B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Problem 2.2 - Base case" sheetId="1" r:id="rId1"/>
@@ -471,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1200,7 +1200,7 @@
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added venv, reorganized task 2
</commit_message>
<xml_diff>
--- a/Task2/Input/Problem 2 data.xlsx
+++ b/Task2/Input/Problem 2 data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frederikedvardsen/Desktop/4. semester/TET4185 Kraftmarkeder, ressurs og miljø/Prosjekt/Task2/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60AF2A11-3EDB-5946-8018-C44056679608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB91CEFC-7664-8B46-8E4D-DF3D5D9FD774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="37">
   <si>
     <t>Generator Data</t>
   </si>
@@ -138,13 +138,25 @@
   </si>
   <si>
     <t>CO2 emission [kg/MWh]</t>
+  </si>
+  <si>
+    <t>Node 4</t>
+  </si>
+  <si>
+    <t>Line 2-4</t>
+  </si>
+  <si>
+    <t>Line 3-4</t>
+  </si>
+  <si>
+    <t>Load 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,6 +168,12 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -469,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -566,7 +584,7 @@
         <v>1000</v>
       </c>
       <c r="C4">
-        <v>300</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -578,7 +596,7 @@
         <v>14</v>
       </c>
       <c r="K4">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="L4" t="s">
         <v>13</v>
@@ -587,10 +605,10 @@
         <v>15</v>
       </c>
       <c r="Q4">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="R4">
-        <v>-20</v>
+        <v>-19.84</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -601,10 +619,10 @@
         <v>1000</v>
       </c>
       <c r="C5">
-        <v>1000</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -613,7 +631,7 @@
         <v>18</v>
       </c>
       <c r="K5">
-        <v>200</v>
+        <v>170</v>
       </c>
       <c r="L5" t="s">
         <v>17</v>
@@ -622,45 +640,50 @@
         <v>19</v>
       </c>
       <c r="Q5">
-        <v>500</v>
+        <v>10000</v>
       </c>
       <c r="R5">
-        <v>-10</v>
+        <v>-26.88</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6">
-        <v>1000</v>
-      </c>
-      <c r="C6">
-        <v>600</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="b">
-        <v>0</v>
-      </c>
       <c r="J6" t="s">
         <v>22</v>
       </c>
       <c r="K6">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="L6" t="s">
         <v>21</v>
       </c>
       <c r="P6" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="Q6">
+        <v>10000</v>
+      </c>
+      <c r="R6">
+        <v>-26.88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="J7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7">
+        <v>80</v>
+      </c>
+      <c r="L7" t="s">
+        <v>33</v>
+      </c>
+      <c r="P7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7">
         <v>100</v>
       </c>
-      <c r="R6">
-        <v>-30</v>
+      <c r="R7">
+        <v>-15.72</v>
       </c>
     </row>
   </sheetData>
@@ -669,6 +692,7 @@
     <mergeCell ref="J1:L2"/>
     <mergeCell ref="P1:S2"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Treat 4d and 4e differently
</commit_message>
<xml_diff>
--- a/Task2/Input/Problem 2 data.xlsx
+++ b/Task2/Input/Problem 2 data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frederikedvardsen/Desktop/4. semester/TET4185 Kraftmarkeder, ressurs og miljø/Prosjekt/Task2/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB91CEFC-7664-8B46-8E4D-DF3D5D9FD774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2528A93-087B-7947-952B-EBCD7302B9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Problem 2.2 - Base case" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="33">
   <si>
     <t>Generator Data</t>
   </si>
@@ -138,25 +138,13 @@
   </si>
   <si>
     <t>CO2 emission [kg/MWh]</t>
-  </si>
-  <si>
-    <t>Node 4</t>
-  </si>
-  <si>
-    <t>Line 2-4</t>
-  </si>
-  <si>
-    <t>Line 3-4</t>
-  </si>
-  <si>
-    <t>Load 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,12 +156,6 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -487,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -584,7 +566,7 @@
         <v>1000</v>
       </c>
       <c r="C4">
-        <v>50</v>
+        <v>300</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -596,7 +578,7 @@
         <v>14</v>
       </c>
       <c r="K4">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="L4" t="s">
         <v>13</v>
@@ -605,10 +587,10 @@
         <v>15</v>
       </c>
       <c r="Q4">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="R4">
-        <v>-19.84</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -619,10 +601,10 @@
         <v>1000</v>
       </c>
       <c r="C5">
-        <v>45</v>
+        <v>1000</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -631,7 +613,7 @@
         <v>18</v>
       </c>
       <c r="K5">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="L5" t="s">
         <v>17</v>
@@ -640,50 +622,45 @@
         <v>19</v>
       </c>
       <c r="Q5">
-        <v>10000</v>
+        <v>500</v>
       </c>
       <c r="R5">
-        <v>-26.88</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>1000</v>
+      </c>
+      <c r="C6">
+        <v>600</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
       <c r="J6" t="s">
         <v>22</v>
       </c>
       <c r="K6">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="L6" t="s">
         <v>21</v>
       </c>
       <c r="P6" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="Q6">
-        <v>10000</v>
+        <v>100</v>
       </c>
       <c r="R6">
-        <v>-26.88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="J7" t="s">
-        <v>36</v>
-      </c>
-      <c r="K7">
-        <v>80</v>
-      </c>
-      <c r="L7" t="s">
-        <v>33</v>
-      </c>
-      <c r="P7" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q7">
-        <v>100</v>
-      </c>
-      <c r="R7">
-        <v>-15.72</v>
+        <v>-30</v>
       </c>
     </row>
   </sheetData>
@@ -692,7 +669,6 @@
     <mergeCell ref="J1:L2"/>
     <mergeCell ref="P1:S2"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -702,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80207373-1C33-4BD6-BF3C-68D230C21681}">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -919,7 +895,7 @@
         <v>1000</v>
       </c>
       <c r="C8">
-        <v>600</v>
+        <v>1000</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
@@ -944,7 +920,7 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1223,8 +1199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9840F038-FFE4-46D4-95DA-D10F47E3A31C}">
   <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Implemented CES for task 2-5
</commit_message>
<xml_diff>
--- a/Task2/Input/Problem 2 data.xlsx
+++ b/Task2/Input/Problem 2 data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frederikedvardsen/Desktop/4. semester/TET4185 Kraftmarkeder, ressurs og miljø/Prosjekt/Task2/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2528A93-087B-7947-952B-EBCD7302B9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3409F8-1E17-EA40-9864-1F69149F43D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -472,7 +472,7 @@
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -679,7 +679,7 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -895,7 +895,7 @@
         <v>1000</v>
       </c>
       <c r="C8">
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
@@ -920,7 +920,7 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Properly implement CES/CAT mechanisms for 2-5
</commit_message>
<xml_diff>
--- a/Task2/Input/Problem 2 data.xlsx
+++ b/Task2/Input/Problem 2 data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frederikedvardsen/Desktop/4. semester/TET4185 Kraftmarkeder, ressurs og miljø/Prosjekt/Task2/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3409F8-1E17-EA40-9864-1F69149F43D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226D70CE-221A-6A47-954F-54C7CCD79CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Problem 2.2 - Base case" sheetId="1" r:id="rId1"/>
@@ -471,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -613,7 +613,7 @@
         <v>18</v>
       </c>
       <c r="K5">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="L5" t="s">
         <v>17</v>
@@ -678,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80207373-1C33-4BD6-BF3C-68D230C21681}">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -920,7 +920,7 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1199,8 +1199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9840F038-FFE4-46D4-95DA-D10F47E3A31C}">
   <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Prepare for delivery of Task 2
</commit_message>
<xml_diff>
--- a/Task2/Input/Problem 2 data.xlsx
+++ b/Task2/Input/Problem 2 data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27504"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frederikedvardsen/Desktop/4. semester/TET4185 Kraftmarkeder, ressurs og miljø/Prosjekt/Task2/Input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emildi/Dropbox (MIT)/1_Projects/1. PhD/Scientific assistantship/Final Project 2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF2A0C5-8AE3-064D-BAE8-AFC443DA11EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="13_ncr:1_{0108DC76-F60C-964F-BF8B-76BF26296CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5E3CA89-DA16-47E4-BE37-30D47D67AB08}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21240" firstSheet="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Problem 2.2 - Base case" sheetId="1" r:id="rId1"/>
@@ -144,7 +144,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,25 +471,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.83203125" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14" customWidth="1"/>
-    <col min="19" max="19" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -509,7 +509,7 @@
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -523,7 +523,7 @@
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -558,7 +558,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -593,7 +593,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -628,7 +628,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -657,7 +657,7 @@
         <v>23</v>
       </c>
       <c r="Q6">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R6">
         <v>-30</v>
@@ -679,24 +679,24 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -716,7 +716,7 @@
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -730,7 +730,7 @@
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -765,7 +765,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -800,7 +800,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -835,7 +835,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -864,13 +864,13 @@
         <v>23</v>
       </c>
       <c r="Q6">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R6">
         <v>-30</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -887,7 +887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -895,7 +895,7 @@
         <v>1000</v>
       </c>
       <c r="C8">
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
@@ -920,33 +920,33 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="9.1640625"/>
+    <col min="6" max="10" width="9.140625"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="9.1640625"/>
-    <col min="16" max="16" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="9.140625"/>
+    <col min="16" max="16" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
       <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
@@ -956,26 +956,26 @@
       <c r="P1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-    </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1199,22 +1199,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9840F038-FFE4-46D4-95DA-D10F47E3A31C}">
   <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="23.5" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-    <col min="7" max="10" width="8.1640625" customWidth="1"/>
-    <col min="11" max="14" width="16.6640625" customWidth="1"/>
-    <col min="15" max="17" width="8.1640625" customWidth="1"/>
-    <col min="18" max="21" width="16.6640625" customWidth="1"/>
+    <col min="1" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="10" width="8.140625" customWidth="1"/>
+    <col min="11" max="14" width="16.7109375" customWidth="1"/>
+    <col min="15" max="17" width="8.140625" customWidth="1"/>
+    <col min="18" max="21" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1236,7 +1236,7 @@
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1252,7 +1252,7 @@
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21">
       <c r="A8" t="s">
         <v>20</v>
       </c>

</xml_diff>